<commit_message>
LCA includes direct non-biogenic emissions
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/HP/data/HP_stacked_area_contributions_2021.2.2-21.32.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/HP/data/HP_stacked_area_contributions_2021.2.2-21.32.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\HP\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5C25C2-5FF3-4C72-A6B2-DAE57357B7B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1152" yWindow="0" windowWidth="19308" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heat utility" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,18 @@
     <sheet name="Installed utility" sheetId="3" r:id="rId3"/>
     <sheet name="MPSP" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -46,8 +63,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +127,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -156,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,9 +213,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,6 +265,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,14 +458,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>15</v>
       </c>
@@ -438,22 +499,22 @@
         <v>11.50355392604154</v>
       </c>
       <c r="D2">
-        <v>14.08310841649367</v>
+        <v>14.083108416493671</v>
       </c>
       <c r="E2">
-        <v>81.94723847456791</v>
+        <v>81.947238474567911</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>-16.85040784091784</v>
+        <v>-16.850407840917839</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>22.10526315789474</v>
       </c>
@@ -464,50 +525,50 @@
         <v>11.14679945896348</v>
       </c>
       <c r="D3">
-        <v>11.07848020660886</v>
+        <v>11.078480206608861</v>
       </c>
       <c r="E3">
-        <v>58.56510519460035</v>
+        <v>58.565105194600349</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>-16.65641616486971</v>
+        <v>-16.656416164869711</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>29.21052631578947</v>
+        <v>29.210526315789469</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>10.96689286113248</v>
+        <v>10.966892861132481</v>
       </c>
       <c r="D4">
-        <v>9.60232015590131</v>
+        <v>9.6023201559013103</v>
       </c>
       <c r="E4">
-        <v>47.09509483626753</v>
+        <v>47.095094836267528</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>-16.43562658681435</v>
+        <v>-16.435626586814351</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>36.31578947368421</v>
+        <v>36.315789473684212</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -516,33 +577,33 @@
         <v>10.85852753078305</v>
       </c>
       <c r="D5">
-        <v>8.725546409623959</v>
+        <v>8.7255464096239592</v>
       </c>
       <c r="E5">
-        <v>40.28833796762586</v>
+        <v>40.288337967625857</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>-16.30203817303143</v>
+        <v>-16.302038173031431</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>43.42105263157895</v>
+        <v>43.421052631578952</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>10.78606426827612</v>
+        <v>10.786064268276119</v>
       </c>
       <c r="D6">
-        <v>8.144827550458807</v>
+        <v>8.1448275504588068</v>
       </c>
       <c r="E6">
         <v>35.78371596915715</v>
@@ -551,50 +612,50 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>-16.19935511540499</v>
+        <v>-16.199355115404991</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>50.52631578947368</v>
+        <v>50.526315789473678</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>10.73435451394307</v>
+        <v>10.734354513943069</v>
       </c>
       <c r="D7">
-        <v>7.761957495075561</v>
+        <v>7.7619574950755608</v>
       </c>
       <c r="E7">
-        <v>32.58596604072194</v>
+        <v>32.585966040721942</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>-18.0053440268824</v>
+        <v>-18.005344026882401</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>57.63157894736842</v>
+        <v>57.631578947368418</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>10.69555856930418</v>
+        <v>10.695558569304181</v>
       </c>
       <c r="D8">
-        <v>8.033500192578236</v>
+        <v>8.0335001925782361</v>
       </c>
       <c r="E8">
         <v>30.19879790238296</v>
@@ -603,13 +664,13 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>-17.89097567459149</v>
+        <v>-17.890975674591491</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>64.73684210526315</v>
       </c>
@@ -620,22 +681,22 @@
         <v>10.66558530277752</v>
       </c>
       <c r="D9">
-        <v>7.333836785113922</v>
+        <v>7.3338367851139221</v>
       </c>
       <c r="E9">
-        <v>28.35727162512268</v>
+        <v>28.357271625122682</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>-17.5628278759055</v>
+        <v>-17.562827875905501</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>71.84210526315789</v>
       </c>
@@ -646,10 +707,10 @@
         <v>10.6415930007505</v>
       </c>
       <c r="D10">
-        <v>7.357702845850596</v>
+        <v>7.3577028458505964</v>
       </c>
       <c r="E10">
-        <v>26.88576260526239</v>
+        <v>26.885762605262389</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -661,7 +722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>78.94736842105263</v>
       </c>
@@ -675,7 +736,7 @@
         <v>8.113679030478286</v>
       </c>
       <c r="E11">
-        <v>25.6841904418353</v>
+        <v>25.684190441835302</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -687,7 +748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>86.05263157894737</v>
       </c>
@@ -695,7 +756,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>10.60544629635782</v>
+        <v>10.605446296357821</v>
       </c>
       <c r="D12">
         <v>8.743133601586635</v>
@@ -707,13 +768,13 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>-16.46075872738968</v>
+        <v>-16.460758727389681</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>93.15789473684211</v>
       </c>
@@ -721,13 +782,13 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>10.59151400514854</v>
+        <v>10.591514005148539</v>
       </c>
       <c r="D13">
-        <v>9.275335521497698</v>
+        <v>9.2753355214976985</v>
       </c>
       <c r="E13">
-        <v>23.83960941319243</v>
+        <v>23.839609413192431</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -739,9 +800,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>100.2631578947368</v>
+        <v>100.26315789473681</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -750,10 +811,10 @@
         <v>10.57957286411933</v>
       </c>
       <c r="D14">
-        <v>9.730828294902617</v>
+        <v>9.7308282949026168</v>
       </c>
       <c r="E14">
-        <v>23.11676447703333</v>
+        <v>23.116764477033328</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -765,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>107.3684210526316</v>
       </c>
@@ -776,7 +837,7 @@
         <v>10.56921031161075</v>
       </c>
       <c r="D15">
-        <v>10.12539613799781</v>
+        <v>10.125396137997811</v>
       </c>
       <c r="E15">
         <v>22.49105010254576</v>
@@ -791,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>114.4736842105263</v>
       </c>
@@ -802,7 +863,7 @@
         <v>10.56013184076124</v>
       </c>
       <c r="D16">
-        <v>10.47042036092786</v>
+        <v>10.470420360927861</v>
       </c>
       <c r="E16">
         <v>21.94365921285835</v>
@@ -811,13 +872,13 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>-15.35260932361586</v>
+        <v>-15.352609323615861</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>121.5789473684211</v>
       </c>
@@ -831,27 +892,27 @@
         <v>10.77475397399995</v>
       </c>
       <c r="E17">
-        <v>21.46200919771296</v>
+        <v>21.462009197712959</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>-15.06628940871875</v>
+        <v>-15.066289408718751</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>128.6842105263158</v>
+        <v>128.68421052631581</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>10.54502139314791</v>
+        <v>10.545021393147911</v>
       </c>
       <c r="D18">
         <v>11.04513614618798</v>
@@ -863,41 +924,41 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>-14.9021461765111</v>
+        <v>-14.902146176511099</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>135.7894736842105</v>
+        <v>135.78947368421049</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>10.5386579011606</v>
+        <v>10.538657901160599</v>
       </c>
       <c r="D19">
-        <v>11.28666523632709</v>
+        <v>11.286665236327091</v>
       </c>
       <c r="E19">
-        <v>20.65278482443494</v>
+        <v>20.652784824434939</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>-16.60242641719138</v>
+        <v>-16.602426417191381</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>142.8947368421053</v>
+        <v>142.89473684210529</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -906,7 +967,7 @@
         <v>10.53293204509569</v>
       </c>
       <c r="D20">
-        <v>11.50411719792067</v>
+        <v>11.504117197920669</v>
       </c>
       <c r="E20">
         <v>20.30970811659256</v>
@@ -921,7 +982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>150</v>
       </c>
@@ -932,7 +993,7 @@
         <v>10.52775113512871</v>
       </c>
       <c r="D21">
-        <v>11.70073354420068</v>
+        <v>11.700733544200681</v>
       </c>
       <c r="E21">
         <v>20.0002871838525</v>
@@ -953,14 +1014,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -983,7 +1046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>15</v>
       </c>
@@ -991,25 +1054,53 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.0003872256452304585</v>
+        <v>3.8722564523045852E-4</v>
       </c>
       <c r="D2">
-        <v>0.0003442064626518277</v>
+        <v>3.4420646265182771E-4</v>
       </c>
       <c r="E2">
-        <v>0.0002269534323408118</v>
+        <v>2.2695343234081181E-4</v>
       </c>
       <c r="F2">
-        <v>0.00161001848098839</v>
+        <v>1.6100184809883899E-3</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>3.673815185101828E-05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>3.6738151851018277E-5</v>
+      </c>
+      <c r="J2">
+        <f>1000000*B2</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>1000*C2</f>
+        <v>0.38722564523045849</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:P17" si="0">1000*D2</f>
+        <v>0.34420646265182769</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>0.22695343234081181</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>1.61001848098839</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="0"/>
+        <v>3.673815185101828E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>22.10526315789474</v>
       </c>
@@ -1017,155 +1108,323 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.0003752167931742164</v>
+        <v>3.752167931742164E-4</v>
       </c>
       <c r="D3">
-        <v>0.0003266060220554576</v>
+        <v>3.2660602205545762E-4</v>
       </c>
       <c r="E3">
-        <v>0.0001597268121957945</v>
+        <v>1.5972681219579449E-4</v>
       </c>
       <c r="F3">
-        <v>0.001058377548251664</v>
+        <v>1.058377548251664E-3</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>2.817198934884202E-05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>2.8171989348842019E-5</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J21" si="1">1000000*B3</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K21" si="2">1000*C3</f>
+        <v>0.37521679317421641</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>0.32660602205545763</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>0.15972681219579449</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>1.058377548251664</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>2.8171989348842019E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>29.21052631578947</v>
+        <v>29.210526315789469</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.0003691608865476013</v>
+        <v>3.6916088654760128E-4</v>
       </c>
       <c r="D4">
-        <v>0.000316967688311923</v>
+        <v>3.16967688311923E-4</v>
       </c>
       <c r="E4">
-        <v>0.0001236876837024412</v>
+        <v>1.2368768370244119E-4</v>
       </c>
       <c r="F4">
-        <v>0.0007878245739695286</v>
+        <v>7.878245739695286E-4</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>2.394950198583497E-05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>2.394950198583497E-5</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0.36916088654760126</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0.31696768831192301</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0.1236876837024412</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>0.78782457396952865</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>2.3949501985834971E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>36.31578947368421</v>
+        <v>36.315789473684212</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.0003655131586150528</v>
+        <v>3.6551315861505282E-4</v>
       </c>
       <c r="D5">
-        <v>0.0003105125634305372</v>
+        <v>3.1051256343053718E-4</v>
       </c>
       <c r="E5">
-        <v>0.0001022812862605214</v>
+        <v>1.022812862605214E-4</v>
       </c>
       <c r="F5">
-        <v>0.0006272794367204915</v>
+        <v>6.2727943672049149E-4</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>2.144113189935863E-05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>2.144113189935863E-5</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>0.36551315861505285</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0.31051256343053718</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0.1022812862605214</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>0.62727943672049147</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>2.1441131899358631E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>43.42105263157895</v>
+        <v>43.421052631578952</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.0003630739442844381</v>
+        <v>3.6307394428443808E-4</v>
       </c>
       <c r="D6">
-        <v>0.0003056455038202714</v>
+        <v>3.0564550382027142E-4</v>
       </c>
       <c r="E6">
-        <v>8.809986489269327E-05</v>
+        <v>8.8099864892693269E-5</v>
       </c>
       <c r="F6">
-        <v>0.0005210089472841363</v>
+        <v>5.2100894728413633E-4</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1.978935814423702E-05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>1.9789358144237021E-5</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0.36307394428443807</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.30564550382027145</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>8.8099864892693266E-2</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0.52100894728413638</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>1.9789358144237022E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>50.52631578947368</v>
+        <v>50.526315789473678</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.0003613333219409482</v>
+        <v>3.6133332194094822E-4</v>
       </c>
       <c r="D7">
-        <v>0.0002988122817812027</v>
+        <v>2.9881228178120273E-4</v>
       </c>
       <c r="E7">
-        <v>7.801430822032043E-05</v>
+        <v>7.801430822032043E-5</v>
       </c>
       <c r="F7">
-        <v>0.0004523116972350077</v>
+        <v>4.5231169723500769E-4</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1.869396865934496E-05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>1.8693968659344961E-5</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0.36133332194094819</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.29881228178120273</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>7.8014308220320433E-2</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0.45231169723500769</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>1.8693968659344962E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>57.63157894736842</v>
+        <v>57.631578947368418</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0.0003600273964159434</v>
+        <v>3.6002739641594338E-4</v>
       </c>
       <c r="D8">
-        <v>0.0002955520395874566</v>
+        <v>2.9555203958745661E-4</v>
       </c>
       <c r="E8">
-        <v>7.047383811924749E-05</v>
+        <v>7.0473838119247494E-5</v>
       </c>
       <c r="F8">
-        <v>0.0004036255239734111</v>
+        <v>4.0362552397341111E-4</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1.789830778602949E-05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>1.7898307786029489E-5</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>0.36002739641594339</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0.29555203958745663</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>7.0473838119247498E-2</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0.40362552397341112</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>1.789830778602949E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>64.73684210526315</v>
       </c>
@@ -1173,25 +1432,53 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0.000359018454522937</v>
+        <v>3.5901845452293699E-4</v>
       </c>
       <c r="D9">
-        <v>0.0002931269705898166</v>
+        <v>2.9312697058981658E-4</v>
       </c>
       <c r="E9">
-        <v>6.462225643109969E-05</v>
+        <v>6.4622256431099695E-5</v>
       </c>
       <c r="F9">
-        <v>0.0003886692173711841</v>
+        <v>3.8866921737118411E-4</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1.752353626473983E-05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>1.752353626473983E-5</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>0.35901845452293696</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0.29312697058981657</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>6.4622256431099701E-2</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>0.38866921737118409</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>1.752353626473983E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>71.84210526315789</v>
       </c>
@@ -1199,25 +1486,53 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0.000358210840224269</v>
+        <v>3.5821084022426899E-4</v>
       </c>
       <c r="D10">
-        <v>0.0002909653394129448</v>
+        <v>2.9096533941294482E-4</v>
       </c>
       <c r="E10">
-        <v>5.99487473414204E-05</v>
+        <v>5.99487473414204E-5</v>
       </c>
       <c r="F10">
-        <v>0.0003878586048501843</v>
+        <v>3.878586048501843E-4</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1.735187983626934E-05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>1.7351879836269339E-5</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>0.35821084022426897</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0.29096533941294483</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>5.9948747341420403E-2</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0.38785860485018431</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>1.7351879836269339E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>78.94736842105263</v>
       </c>
@@ -1225,25 +1540,53 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0.0003575477302045621</v>
+        <v>3.5754773020456212E-4</v>
       </c>
       <c r="D11">
-        <v>0.0002886334004909299</v>
+        <v>2.8863340049092992E-4</v>
       </c>
       <c r="E11">
-        <v>5.612957874215018E-05</v>
+        <v>5.6129578742150182E-5</v>
       </c>
       <c r="F11">
-        <v>0.0003871783863089532</v>
+        <v>3.8717838630895321E-4</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>1.721455445657125E-05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>1.721455445657125E-5</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>0.3575477302045621</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0.28863340049092989</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>5.6129578742150181E-2</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>0.38717838630895318</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>1.721455445657125E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>86.05263157894737</v>
       </c>
@@ -1251,25 +1594,53 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0.0003569940918153673</v>
+        <v>3.5699409181536728E-4</v>
       </c>
       <c r="D12">
-        <v>0.0002864008347028077</v>
+        <v>2.8640083470280771E-4</v>
       </c>
       <c r="E12">
-        <v>5.294939601283739E-05</v>
+        <v>5.2949396012837388E-5</v>
       </c>
       <c r="F12">
-        <v>0.000386600553041828</v>
+        <v>3.8660055304182801E-4</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>1.71018495761177E-05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>1.7101849576117699E-5</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>0.35699409181536729</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0.28640083470280769</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>5.2949396012837387E-2</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0.386600553041828</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>1.7101849576117698E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>93.15789473684211</v>
       </c>
@@ -1277,51 +1648,107 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0.0003565251114907135</v>
+        <v>3.5652511149071348E-4</v>
       </c>
       <c r="D13">
-        <v>0.0002842464116530268</v>
+        <v>2.8424641165302681E-4</v>
       </c>
       <c r="E13">
-        <v>5.026003769769972E-05</v>
+        <v>5.0260037697699722E-5</v>
       </c>
       <c r="F13">
-        <v>0.0003861103816539786</v>
+        <v>3.861103816539786E-4</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>1.700755628995869E-05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>1.7007556289958689E-5</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>0.35652511149071348</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0.28424641165302683</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>5.0260037697699725E-2</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0.3861103816539786</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>1.7007556289958689E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>100.2631578947368</v>
+        <v>100.26315789473681</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0.0003561231560540599</v>
+        <v>3.5612315605405988E-4</v>
       </c>
       <c r="D14">
-        <v>0.000282165906120312</v>
+        <v>2.82165906120312E-4</v>
       </c>
       <c r="E14">
-        <v>4.795748584526949E-05</v>
+        <v>4.7957485845269487E-5</v>
       </c>
       <c r="F14">
-        <v>0.0003856938100925877</v>
+        <v>3.8569381009258768E-4</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>1.692749337589308E-05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>1.6927493375893081E-5</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>0.35612315605405986</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0.282165906120312</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>4.7957485845269487E-2</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.38569381009258769</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>1.6927493375893079E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>107.3684210526316</v>
       </c>
@@ -1329,25 +1756,53 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0.0003557743381054026</v>
+        <v>3.5577433810540262E-4</v>
       </c>
       <c r="D15">
-        <v>0.0002801328480448243</v>
+        <v>2.801328480448243E-4</v>
       </c>
       <c r="E15">
-        <v>4.59622131812761E-05</v>
+        <v>4.5962213181276097E-5</v>
       </c>
       <c r="F15">
-        <v>0.0003853260591749052</v>
+        <v>3.8532605917490517E-4</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>1.685856012236702E-05</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>1.685856012236702E-5</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>0.3557743381054026</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0.2801328480448243</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>4.59622131812761E-2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0.3853260591749052</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>1.6858560122367021E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>114.4736842105263</v>
       </c>
@@ -1355,25 +1810,53 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0.0003554687441336425</v>
+        <v>3.5546874413364251E-4</v>
       </c>
       <c r="D16">
-        <v>0.0002781411002453163</v>
+        <v>2.7814110024531631E-4</v>
       </c>
       <c r="E16">
-        <v>4.421660577185379E-05</v>
+        <v>4.4216605771853792E-5</v>
       </c>
       <c r="F16">
-        <v>0.0003850091360148497</v>
+        <v>3.8500913601484968E-4</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>1.679857199254504E-05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>1.6798571992545042E-5</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>0.35546874413364249</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.2781411002453163</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>4.4216605771853795E-2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0.38500913601484965</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>1.6798571992545041E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>121.5789473684211</v>
       </c>
@@ -1381,103 +1864,215 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0.0003551995979792948</v>
+        <v>3.5519959797929482E-4</v>
       </c>
       <c r="D17">
-        <v>0.0002761821174807587</v>
+        <v>2.7618211748075872E-4</v>
       </c>
       <c r="E17">
-        <v>4.267662061553691E-05</v>
+        <v>4.267662061553691E-5</v>
       </c>
       <c r="F17">
-        <v>0.0003847198048055777</v>
+        <v>3.847198048055777E-4</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>1.674591422783454E-05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>1.6745914227834539E-5</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>0.35519959797929485</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>0.27618211748075872</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>4.2676620615536912E-2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>0.38471980480557771</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>1.674591422783454E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>128.6842105263158</v>
+        <v>128.68421052631581</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>0.0003549601054236904</v>
+        <v>3.5496010542369042E-4</v>
       </c>
       <c r="D18">
-        <v>0.0002742515113519627</v>
+        <v>2.7425151135196271E-4</v>
       </c>
       <c r="E18">
-        <v>4.130765649045757E-05</v>
+        <v>4.1307656490457573E-5</v>
       </c>
       <c r="F18">
-        <v>0.0003844728422944018</v>
+        <v>3.8447284229440178E-4</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>1.66992750321846E-05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>1.6699275032184599E-5</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>0.35496010542369044</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L21" si="3">1000*D18</f>
+        <v>0.27425151135196274</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M21" si="4">1000*E18</f>
+        <v>4.1307656490457575E-2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ref="N18:N21" si="5">1000*F18</f>
+        <v>0.38447284229440176</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18:O21" si="6">1000*G18</f>
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18:P21" si="7">1000*H18</f>
+        <v>1.6699275032184598E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>135.7894736842105</v>
+        <v>135.78947368421049</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>0.0003547459014213972</v>
+        <v>3.5474590142139722E-4</v>
       </c>
       <c r="D19">
-        <v>0.0002723576247552986</v>
+        <v>2.7235762475529858E-4</v>
       </c>
       <c r="E19">
-        <v>4.00856949464809E-05</v>
+        <v>4.0085694946480902E-5</v>
       </c>
       <c r="F19">
-        <v>0.0003842424228205818</v>
+        <v>3.8424242282058179E-4</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>1.665077755571704E-05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>1.665077755571704E-5</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>0.35474590142139723</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>0.27235762475529857</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>4.0085694946480899E-2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>0.3842424228205818</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="7"/>
+        <v>1.665077755571704E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>142.8947368421053</v>
+        <v>142.89473684210529</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0.0003545531611322441</v>
+        <v>3.5455316113224412E-4</v>
       </c>
       <c r="D20">
-        <v>0.0002704770651192971</v>
+        <v>2.7047706511929709E-4</v>
       </c>
       <c r="E20">
-        <v>3.899444410490522E-05</v>
+        <v>3.8994444104905221E-5</v>
       </c>
       <c r="F20">
-        <v>0.0003840380637552642</v>
+        <v>3.8403806375526421E-4</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>1.662100362321954E-05</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>1.6621003623219542E-5</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>0.35455316113224411</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>0.27047706511929709</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>3.899444410490522E-2</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="5"/>
+        <v>0.38403806375526423</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="7"/>
+        <v>1.6621003623219541E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>150</v>
       </c>
@@ -1485,22 +2080,50 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0.0003543787644876567</v>
+        <v>3.5437876448765669E-4</v>
       </c>
       <c r="D21">
-        <v>0.0002686167842194866</v>
+        <v>2.6861678421948661E-4</v>
       </c>
       <c r="E21">
-        <v>3.800769833414063E-05</v>
+        <v>3.8007698334140633E-5</v>
       </c>
       <c r="F21">
-        <v>0.0003838516824468226</v>
+        <v>3.8385168244682263E-4</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>1.658738671688876E-05</v>
+        <v>1.6587386716888759E-5</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="2"/>
+        <v>0.35437876448765671</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>0.26861678421948659</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>3.8007698334140631E-2</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="5"/>
+        <v>0.38385168244682261</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="7"/>
+        <v>1.6587386716888759E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1509,14 +2132,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1539,7 +2162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>15</v>
       </c>
@@ -1547,25 +2170,25 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.002167766828749792</v>
+        <v>2.1677668287497921E-3</v>
       </c>
       <c r="D2">
-        <v>0.006530349835498306</v>
+        <v>6.5303498354983064E-3</v>
       </c>
       <c r="E2">
-        <v>0.002249922801481541</v>
+        <v>2.249922801481541E-3</v>
       </c>
       <c r="F2">
-        <v>0.006839755194457993</v>
+        <v>6.8397551944579934E-3</v>
       </c>
       <c r="G2">
-        <v>0.0001531406747044049</v>
+        <v>1.5314067470440491E-4</v>
       </c>
       <c r="H2">
-        <v>0.000627611633494326</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>6.2761163349432604E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>22.10526315789474</v>
       </c>
@@ -1573,155 +2196,155 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.002100538865639511</v>
+        <v>2.1005388656395109E-3</v>
       </c>
       <c r="D3">
-        <v>0.006165215859344013</v>
+        <v>6.1652158593440134E-3</v>
       </c>
       <c r="E3">
-        <v>0.001991980500041313</v>
+        <v>1.991980500041313E-3</v>
       </c>
       <c r="F3">
-        <v>0.005244404401226702</v>
+        <v>5.2444044012267023E-3</v>
       </c>
       <c r="G3">
-        <v>0.0001659683453514759</v>
+        <v>1.6596834535147591E-4</v>
       </c>
       <c r="H3">
-        <v>0.000575433591667158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>5.7543359166715795E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>29.21052631578947</v>
+        <v>29.210526315789469</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.002066636685707042</v>
+        <v>2.0666366857070421E-3</v>
       </c>
       <c r="D4">
-        <v>0.005962364834719741</v>
+        <v>5.9623648347197408E-3</v>
       </c>
       <c r="E4">
-        <v>0.00186298850069808</v>
+        <v>1.8629885006980801E-3</v>
       </c>
       <c r="F4">
-        <v>0.00436154784893357</v>
+        <v>4.3615478489335696E-3</v>
       </c>
       <c r="G4">
-        <v>0.0001697034473036295</v>
+        <v>1.6970344730362949E-4</v>
       </c>
       <c r="H4">
-        <v>0.0005477134780631895</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>5.4771347806318953E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>36.31578947368421</v>
+        <v>36.315789473684212</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.002046215973113724</v>
+        <v>2.0462159731137238E-3</v>
       </c>
       <c r="D5">
-        <v>0.005827156045441676</v>
+        <v>5.8271560454416756E-3</v>
       </c>
       <c r="E5">
-        <v>0.001788068165903393</v>
+        <v>1.7880681659033931E-3</v>
       </c>
       <c r="F5">
-        <v>0.003787425829348949</v>
+        <v>3.787425829348949E-3</v>
       </c>
       <c r="G5">
-        <v>0.0002674936636189461</v>
+        <v>2.6749366361894609E-4</v>
       </c>
       <c r="H5">
-        <v>0.0005302678957404387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>5.302678957404387E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>43.42105263157895</v>
+        <v>43.421052631578952</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.002032560762056307</v>
+        <v>2.032560762056307E-3</v>
       </c>
       <c r="D6">
-        <v>0.005726624124538416</v>
+        <v>5.7266241245384156E-3</v>
       </c>
       <c r="E6">
-        <v>0.001738505673559419</v>
+        <v>1.738505673559419E-3</v>
       </c>
       <c r="F6">
-        <v>0.003378164342992467</v>
+        <v>3.3781643429924668E-3</v>
       </c>
       <c r="G6">
-        <v>0.0002008178468657216</v>
+        <v>2.0081784686572159E-4</v>
       </c>
       <c r="H6">
-        <v>0.0005182001624280995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>5.1820016242809953E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>50.52631578947368</v>
+        <v>50.526315789473678</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.002022816409059816</v>
+        <v>2.0228164090598162E-3</v>
       </c>
       <c r="D7">
-        <v>0.005649589029825742</v>
+        <v>5.6495890298257417E-3</v>
       </c>
       <c r="E7">
-        <v>0.001702667343185072</v>
+        <v>1.7026673431850721E-3</v>
       </c>
       <c r="F7">
-        <v>0.003096821202503146</v>
+        <v>3.0968212025031458E-3</v>
       </c>
       <c r="G7">
-        <v>0.0001882414883598983</v>
+        <v>1.882414883598983E-4</v>
       </c>
       <c r="H7">
-        <v>0.0005094704444058106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>5.0947044440581059E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>57.63157894736842</v>
+        <v>57.631578947368418</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0.002015505576040597</v>
+        <v>2.0155055760405971E-3</v>
       </c>
       <c r="D8">
-        <v>0.005585720511243937</v>
+        <v>5.5857205112439367E-3</v>
       </c>
       <c r="E8">
-        <v>0.001675842802225738</v>
+        <v>1.675842802225738E-3</v>
       </c>
       <c r="F8">
-        <v>0.002887694333224471</v>
+        <v>2.8876943332244711E-3</v>
       </c>
       <c r="G8">
-        <v>0.0001771527916982724</v>
+        <v>1.771527916982724E-4</v>
       </c>
       <c r="H8">
-        <v>0.0005027857605359855</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>5.0278576053598549E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>64.73684210526315</v>
       </c>
@@ -1729,25 +2352,25 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0.002009857316959485</v>
+        <v>2.009857316959485E-3</v>
       </c>
       <c r="D9">
-        <v>0.005536743590759143</v>
+        <v>5.5367435907591432E-3</v>
       </c>
       <c r="E9">
-        <v>0.001654721752050455</v>
+        <v>1.654721752050455E-3</v>
       </c>
       <c r="F9">
-        <v>0.002819709908894554</v>
+        <v>2.8197099088945539E-3</v>
       </c>
       <c r="G9">
-        <v>0.0001562619838559983</v>
+        <v>1.5626198385599831E-4</v>
       </c>
       <c r="H9">
-        <v>0.0004980661258025936</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>4.9806612580259363E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>71.84210526315789</v>
       </c>
@@ -1755,25 +2378,25 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0.002005336130131872</v>
+        <v>2.0053361301318722E-3</v>
       </c>
       <c r="D10">
-        <v>0.005498715854744428</v>
+        <v>5.4987158547444284E-3</v>
       </c>
       <c r="E10">
-        <v>0.0016375197854672</v>
+        <v>1.6375197854672E-3</v>
       </c>
       <c r="F10">
-        <v>0.002813614312285931</v>
+        <v>2.8136143122859309E-3</v>
       </c>
       <c r="G10">
-        <v>0.000165361101075332</v>
+        <v>1.6536110107533199E-4</v>
       </c>
       <c r="H10">
-        <v>0.0004946423976163881</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>4.9464239761638806E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>78.94736842105263</v>
       </c>
@@ -1781,25 +2404,25 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0.002001623907241191</v>
+        <v>2.0016239072411911E-3</v>
       </c>
       <c r="D11">
-        <v>0.00545899981266379</v>
+        <v>5.4589998126637904E-3</v>
       </c>
       <c r="E11">
-        <v>0.001623251827801891</v>
+        <v>1.6232518278018911E-3</v>
       </c>
       <c r="F11">
-        <v>0.002808573892519922</v>
+        <v>2.8085738925199221E-3</v>
       </c>
       <c r="G11">
-        <v>0.0001558009560096732</v>
+        <v>1.5580095600967319E-4</v>
       </c>
       <c r="H11">
-        <v>0.0004918835623840472</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>4.9188356238404724E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>86.05263157894737</v>
       </c>
@@ -1807,25 +2430,25 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0.001998524528494905</v>
+        <v>1.9985245284949052E-3</v>
       </c>
       <c r="D12">
-        <v>0.005420849003940346</v>
+        <v>5.4208490039403456E-3</v>
       </c>
       <c r="E12">
-        <v>0.00161132616766473</v>
+        <v>1.6113261676647299E-3</v>
       </c>
       <c r="F12">
-        <v>0.002804322402694678</v>
+        <v>2.8043224026946781E-3</v>
       </c>
       <c r="G12">
-        <v>0.0001498714967816229</v>
+        <v>1.4987149678162291E-4</v>
       </c>
       <c r="H12">
-        <v>0.000489588488432685</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>4.8958848843268503E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>93.15789473684211</v>
       </c>
@@ -1833,51 +2456,51 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0.001995899082573837</v>
+        <v>1.9958990825738369E-3</v>
       </c>
       <c r="D13">
-        <v>0.005270693337413722</v>
+        <v>5.2706933374137219E-3</v>
       </c>
       <c r="E13">
-        <v>0.00160820401756424</v>
+        <v>1.60820401756424E-3</v>
       </c>
       <c r="F13">
-        <v>0.002800717977639085</v>
+        <v>2.800717977639085E-3</v>
       </c>
       <c r="G13">
-        <v>0.0001459023093046844</v>
+        <v>1.459023093046844E-4</v>
       </c>
       <c r="H13">
-        <v>0.0004876440022469438</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>4.8764400224694381E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>100.2631578947368</v>
+        <v>100.26315789473681</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0.001993648855419015</v>
+        <v>1.9936488554190149E-3</v>
       </c>
       <c r="D14">
-        <v>0.005236478017636781</v>
+        <v>5.2364780176367811E-3</v>
       </c>
       <c r="E14">
-        <v>0.001598767286687886</v>
+        <v>1.598767286687886E-3</v>
       </c>
       <c r="F14">
-        <v>0.002797644130844039</v>
+        <v>2.7976441308440389E-3</v>
       </c>
       <c r="G14">
-        <v>0.0001451424304688874</v>
+        <v>1.4514243046888741E-4</v>
       </c>
       <c r="H14">
-        <v>0.0004859585262577853</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>4.8595852625778533E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>107.3684210526316</v>
       </c>
@@ -1885,25 +2508,25 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0.001991696102579813</v>
+        <v>1.991696102579813E-3</v>
       </c>
       <c r="D15">
-        <v>0.005203429455183262</v>
+        <v>5.2034294551832616E-3</v>
       </c>
       <c r="E15">
-        <v>0.001589795879633124</v>
+        <v>1.5897958796331239E-3</v>
       </c>
       <c r="F15">
-        <v>0.002794949401726256</v>
+        <v>2.7949494017262561E-3</v>
       </c>
       <c r="G15">
-        <v>0.0001445435348166689</v>
+        <v>1.4454353481666891E-4</v>
       </c>
       <c r="H15">
-        <v>0.0004845053102473441</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>4.8450531024734407E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>114.4736842105263</v>
       </c>
@@ -1911,25 +2534,25 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0.001989985326232739</v>
+        <v>1.9899853262327388E-3</v>
       </c>
       <c r="D16">
-        <v>0.005171224895659594</v>
+        <v>5.1712248956595937E-3</v>
       </c>
       <c r="E16">
-        <v>0.001582447512266088</v>
+        <v>1.5824475122660879E-3</v>
       </c>
       <c r="F16">
-        <v>0.00279261149371498</v>
+        <v>2.7926114937149799E-3</v>
       </c>
       <c r="G16">
-        <v>0.0001329436122812582</v>
+        <v>1.329436122812582E-4</v>
       </c>
       <c r="H16">
-        <v>0.0004832105468485399</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>4.832105468485399E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>121.5789473684211</v>
       </c>
@@ -1937,103 +2560,103 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0.0019884785920779</v>
+        <v>1.9884785920778998E-3</v>
       </c>
       <c r="D17">
-        <v>0.005139800406486532</v>
+        <v>5.1398004064865319E-3</v>
       </c>
       <c r="E17">
-        <v>0.001575939378177316</v>
+        <v>1.575939378177316E-3</v>
       </c>
       <c r="F17">
-        <v>0.002790507941886016</v>
+        <v>2.790507941886016E-3</v>
       </c>
       <c r="G17">
-        <v>0.0001264801470828487</v>
+        <v>1.2648014708284869E-4</v>
       </c>
       <c r="H17">
-        <v>0.0004820617761305691</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>4.8206177613056909E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>128.6842105263158</v>
+        <v>128.68421052631581</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>0.001987137864716465</v>
+        <v>1.987137864716465E-3</v>
       </c>
       <c r="D18">
-        <v>0.005109823948460433</v>
+        <v>5.1098239484604329E-3</v>
       </c>
       <c r="E18">
-        <v>0.001569869337339009</v>
+        <v>1.5698693373390089E-3</v>
       </c>
       <c r="F18">
-        <v>0.002788681860144261</v>
+        <v>2.7886818601442608E-3</v>
       </c>
       <c r="G18">
-        <v>0.0001233165460426045</v>
+        <v>1.2331654604260449E-4</v>
       </c>
       <c r="H18">
-        <v>0.0004810267402129572</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>4.8102674021295718E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>135.7894736842105</v>
+        <v>135.78947368421049</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>0.001985938707748607</v>
+        <v>1.9859387077486071E-3</v>
       </c>
       <c r="D19">
-        <v>0.005079810379052284</v>
+        <v>5.0798103790522841E-3</v>
       </c>
       <c r="E19">
-        <v>0.001564615208652305</v>
+        <v>1.564615208652305E-3</v>
       </c>
       <c r="F19">
-        <v>0.002787007036697652</v>
+        <v>2.7870070366976521E-3</v>
       </c>
       <c r="G19">
-        <v>0.0001240772340404801</v>
+        <v>1.2407723404048011E-4</v>
       </c>
       <c r="H19">
-        <v>0.0004800639102287919</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>4.8006391022879189E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>142.8947368421053</v>
+        <v>142.89473684210529</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0.001984859708951896</v>
+        <v>1.9848597089518962E-3</v>
       </c>
       <c r="D20">
-        <v>0.005050163169468374</v>
+        <v>5.0501631694683741E-3</v>
       </c>
       <c r="E20">
-        <v>0.00155972422232806</v>
+        <v>1.55972422232806E-3</v>
       </c>
       <c r="F20">
-        <v>0.002785512980785582</v>
+        <v>2.7855129807855821E-3</v>
       </c>
       <c r="G20">
-        <v>0.0001062136949604821</v>
+        <v>1.062136949604821E-4</v>
       </c>
       <c r="H20">
-        <v>0.0004792491151907689</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>4.7924911519076888E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>150</v>
       </c>
@@ -2041,22 +2664,22 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0.001983883401556659</v>
+        <v>1.9838834015566591E-3</v>
       </c>
       <c r="D21">
-        <v>0.005021043014503669</v>
+        <v>5.0210430145036693E-3</v>
       </c>
       <c r="E21">
-        <v>0.00155526450313459</v>
+        <v>1.55526450313459E-3</v>
       </c>
       <c r="F21">
-        <v>0.00278415469550087</v>
+        <v>2.7841546955008701E-3</v>
       </c>
       <c r="G21">
-        <v>0.000108688121505045</v>
+        <v>1.08688121505045E-4</v>
       </c>
       <c r="H21">
-        <v>0.0004784727806011454</v>
+        <v>4.7847278060114538E-4</v>
       </c>
     </row>
   </sheetData>
@@ -2065,19 +2688,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>15</v>
       </c>
@@ -2085,79 +2708,79 @@
         <v>2262.157343808175</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>22.10526315789474</v>
       </c>
       <c r="B3">
-        <v>1942.32669157269</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>1942.3266915726899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>29.21052631578947</v>
+        <v>29.210526315789469</v>
       </c>
       <c r="B4">
-        <v>1779.209021014775</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>1779.2090210147751</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>36.31578947368421</v>
+        <v>36.315789473684212</v>
       </c>
       <c r="B5">
-        <v>1681.467555658451</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>1681.4675556584509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>43.42105263157895</v>
+        <v>43.421052631578952</v>
       </c>
       <c r="B6">
-        <v>1611.226169952865</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>1611.2261699528649</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>50.52631578947368</v>
+        <v>50.526315789473678</v>
       </c>
       <c r="B7">
         <v>1549.734748417434</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>57.63157894736842</v>
+        <v>57.631578947368418</v>
       </c>
       <c r="B8">
-        <v>1518.449539388541</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>1518.4495393885411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>64.73684210526315</v>
       </c>
       <c r="B9">
-        <v>1488.492028502589</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>1488.4920285025889</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>71.84210526315789</v>
       </c>
       <c r="B10">
-        <v>1477.690076831644</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>1477.6900768316441</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>78.94736842105263</v>
       </c>
       <c r="B11">
-        <v>1469.391045022592</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>1469.3910450225919</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>86.05263157894737</v>
       </c>
@@ -2165,7 +2788,7 @@
         <v>1459.100596321013</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>93.15789473684211</v>
       </c>
@@ -2173,23 +2796,23 @@
         <v>1450.348995037031</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>100.2631578947368</v>
+        <v>100.26315789473681</v>
       </c>
       <c r="B14">
         <v>1445.86930103342</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>107.3684210526316</v>
       </c>
       <c r="B15">
-        <v>1441.898208455479</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>1441.8982084554791</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>114.4736842105263</v>
       </c>
@@ -2197,7 +2820,7 @@
         <v>1439.359931379922</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>121.5789473684211</v>
       </c>
@@ -2205,31 +2828,31 @@
         <v>1436.79076904709</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>128.6842105263158</v>
+        <v>128.68421052631581</v>
       </c>
       <c r="B18">
-        <v>1433.869777116353</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>1433.8697771163529</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>135.7894736842105</v>
+        <v>135.78947368421049</v>
       </c>
       <c r="B19">
         <v>1409.129397918573</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>142.8947368421053</v>
+        <v>142.89473684210529</v>
       </c>
       <c r="B20">
-        <v>1423.257823586444</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>1423.2578235864439</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>150</v>
       </c>

</xml_diff>